<commit_message>
minmax, code cleaning + first results
</commit_message>
<xml_diff>
--- a/PROJECT/PointCould_Classification/trainings.xlsx
+++ b/PROJECT/PointCould_Classification/trainings.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swann\GitHubProjects\IndividualProject\PROJECT\PointCould_Classification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC36DA7D-666E-4791-BA37-59C9C58440D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41B1F325-F37F-4FA2-833A-215F1B19D8EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-114" yWindow="-114" windowWidth="27602" windowHeight="14927" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-114" yWindow="-114" windowWidth="27602" windowHeight="14927" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="3DmFV" sheetId="1" r:id="rId1"/>
     <sheet name="PointTransformer" sheetId="3" r:id="rId2"/>
+    <sheet name="KDE" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="42">
   <si>
     <t>epochs</t>
   </si>
@@ -131,6 +132,27 @@
   </si>
   <si>
     <t>tweaked the random dropout max value from .825 to 0.4  --&gt; Didn't seems to change anything</t>
+  </si>
+  <si>
+    <t>kernel size</t>
+  </si>
+  <si>
+    <t>grid dim</t>
+  </si>
+  <si>
+    <t>results\KDE\wl_da_tt_gd=64_ks=2_epoch=20_5200</t>
+  </si>
+  <si>
+    <t>band width</t>
+  </si>
+  <si>
+    <t>with whitening</t>
+  </si>
+  <si>
+    <t>deeper model</t>
+  </si>
+  <si>
+    <t>24:50:58</t>
   </si>
 </sst>
 </file>
@@ -221,7 +243,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -269,12 +291,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="15">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -613,8 +669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -852,19 +908,19 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="top10" dxfId="9" priority="5" rank="1"/>
+    <cfRule type="top10" dxfId="14" priority="5" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="top10" dxfId="8" priority="4" rank="1"/>
+    <cfRule type="top10" dxfId="13" priority="4" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="top10" dxfId="7" priority="2" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="12" priority="2" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="top10" dxfId="6" priority="3" rank="1"/>
+    <cfRule type="top10" dxfId="11" priority="3" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K1048576">
-    <cfRule type="top10" dxfId="5" priority="1" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="10" priority="1" bottom="1" rank="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="N2" r:id="rId1" xr:uid="{31CF885D-4D4B-49D0-941B-066B53D318A6}"/>
@@ -881,7 +937,7 @@
   <dimension ref="A1:P9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -1326,19 +1382,19 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="top10" dxfId="4" priority="5" rank="1"/>
+    <cfRule type="top10" dxfId="9" priority="5" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="top10" dxfId="3" priority="4" rank="1"/>
+    <cfRule type="top10" dxfId="8" priority="4" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="top10" dxfId="2" priority="3" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="7" priority="3" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="top10" dxfId="1" priority="1" rank="1"/>
+    <cfRule type="top10" dxfId="6" priority="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K1048576">
-    <cfRule type="top10" dxfId="0" priority="2" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="5" priority="2" bottom="1" rank="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="O2" r:id="rId1" xr:uid="{1B75A89D-0C05-438E-96A4-E6EC9D42327C}"/>
@@ -1352,4 +1408,263 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AFD9867-B70B-41BC-9A3A-CD91040257D4}">
+  <dimension ref="A1:Q9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="8" max="9" width="9.140625" style="7"/>
+    <col min="10" max="10" width="9.140625" style="3"/>
+    <col min="11" max="11" width="9.140625" style="9"/>
+    <col min="12" max="12" width="9.140625" style="5"/>
+    <col min="15" max="15" width="10.7109375" style="26" customWidth="1"/>
+    <col min="16" max="16" width="56.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" s="10" customFormat="1" ht="42.8" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="N1" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="O1" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q1" s="10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2">
+        <v>64</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>0.2</v>
+      </c>
+      <c r="H2" s="6">
+        <v>0.80113636363636298</v>
+      </c>
+      <c r="I2" s="7">
+        <v>0.76938593379820897</v>
+      </c>
+      <c r="J2" s="3">
+        <v>4.9005423569016902E-2</v>
+      </c>
+      <c r="K2" s="8">
+        <v>0.79105724088118401</v>
+      </c>
+      <c r="L2" s="5">
+        <v>4.8274670035430199E-2</v>
+      </c>
+      <c r="M2">
+        <v>16</v>
+      </c>
+      <c r="N2">
+        <v>5200</v>
+      </c>
+      <c r="O2" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3">
+        <v>128</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <v>0.2</v>
+      </c>
+      <c r="H3" s="6"/>
+      <c r="K3" s="8"/>
+      <c r="M3">
+        <v>16</v>
+      </c>
+      <c r="N3">
+        <v>5200</v>
+      </c>
+      <c r="P3" s="1"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4">
+        <v>64</v>
+      </c>
+      <c r="F4">
+        <v>4</v>
+      </c>
+      <c r="G4">
+        <v>0.2</v>
+      </c>
+      <c r="H4" s="6"/>
+      <c r="K4" s="8"/>
+      <c r="M4">
+        <v>16</v>
+      </c>
+      <c r="N4">
+        <v>5200</v>
+      </c>
+      <c r="P4" s="1"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5">
+        <v>64</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5">
+        <v>0.4</v>
+      </c>
+      <c r="H5" s="6"/>
+      <c r="K5" s="8"/>
+      <c r="M5">
+        <v>16</v>
+      </c>
+      <c r="N5">
+        <v>5200</v>
+      </c>
+      <c r="P5" s="1"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P6" s="1"/>
+      <c r="Q6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P7" s="1"/>
+      <c r="Q7" s="24" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P8" s="1"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P9" s="1"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="H1:H1048576">
+    <cfRule type="top10" dxfId="4" priority="5" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I1:I1048576">
+    <cfRule type="top10" dxfId="3" priority="4" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J1:J1048576">
+    <cfRule type="top10" dxfId="2" priority="3" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K1:K1048576">
+    <cfRule type="top10" dxfId="1" priority="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L1:L1048576">
+    <cfRule type="top10" dxfId="0" priority="2" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="P2" r:id="rId1" xr:uid="{06379612-5A90-48F1-A974-5BCDF9391FD0}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
globavg + test with kernel size = 4
</commit_message>
<xml_diff>
--- a/PROJECT/PointCould_Classification/trainings.xlsx
+++ b/PROJECT/PointCould_Classification/trainings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swann\GitHubProjects\IndividualProject\PROJECT\PointCould_Classification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41B1F325-F37F-4FA2-833A-215F1B19D8EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECFCADB8-B477-4C5E-B24F-91F88C1B6F7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-114" yWindow="-114" windowWidth="27602" windowHeight="14927" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27488" yWindow="-114" windowWidth="27602" windowHeight="14899" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="3DmFV" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="KDE" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="52">
   <si>
     <t>epochs</t>
   </si>
@@ -146,13 +147,43 @@
     <t>band width</t>
   </si>
   <si>
-    <t>with whitening</t>
-  </si>
-  <si>
-    <t>deeper model</t>
-  </si>
-  <si>
     <t>24:50:58</t>
+  </si>
+  <si>
+    <t>results\KDE\wl_da_tt_gd=64_ks=2_epoch=100_5200</t>
+  </si>
+  <si>
+    <t>13:38:33</t>
+  </si>
+  <si>
+    <t>results\KDE\wl_da_tt_gd=64_ks=2_epoch=20_5200_deep</t>
+  </si>
+  <si>
+    <t>11:43:58</t>
+  </si>
+  <si>
+    <t>model</t>
+  </si>
+  <si>
+    <t>model_deep</t>
+  </si>
+  <si>
+    <t>model_globavg</t>
+  </si>
+  <si>
+    <t>might be too big but interesting to look into deeper models</t>
+  </si>
+  <si>
+    <t>11:45:40</t>
+  </si>
+  <si>
+    <t>results\KDE\wl_da_tt_gd=64_ks=2_epoch=100_5200_globavg</t>
+  </si>
+  <si>
+    <t>went very fast to the best result (epoch 17) but the model is very small.. Might help to go deeper</t>
+  </si>
+  <si>
+    <t>results\KDE\wl_da_tt_gd=64_ks=4_epoch=100_5200_globavg</t>
   </si>
 </sst>
 </file>
@@ -1412,10 +1443,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AFD9867-B70B-41BC-9A3A-CD91040257D4}">
-  <dimension ref="A1:Q9"/>
+  <dimension ref="A1:R12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -1425,11 +1456,12 @@
     <col min="11" max="11" width="9.140625" style="9"/>
     <col min="12" max="12" width="9.140625" style="5"/>
     <col min="15" max="15" width="10.7109375" style="26" customWidth="1"/>
-    <col min="16" max="16" width="56.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.7109375" style="26" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="56.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="55" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="10" customFormat="1" ht="42.8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" s="10" customFormat="1" ht="42.8" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -1475,14 +1507,17 @@
       <c r="O1" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="P1" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="Q1" s="10" t="s">
+      <c r="R1" s="10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>20</v>
       </c>
@@ -1526,15 +1561,18 @@
         <v>5200</v>
       </c>
       <c r="O2" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="P2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="P2" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q2" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="B3" t="s">
         <v>13</v>
@@ -1546,7 +1584,7 @@
         <v>14</v>
       </c>
       <c r="E3">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="F3">
         <v>2</v>
@@ -1554,17 +1592,38 @@
       <c r="G3">
         <v>0.2</v>
       </c>
-      <c r="H3" s="6"/>
-      <c r="K3" s="8"/>
+      <c r="H3" s="6">
+        <v>0.84911616161616099</v>
+      </c>
+      <c r="I3" s="7">
+        <v>0.80872779356216196</v>
+      </c>
+      <c r="J3" s="3">
+        <v>9.2817636639481796E-2</v>
+      </c>
+      <c r="K3" s="8">
+        <v>0.86518147345612095</v>
+      </c>
+      <c r="L3" s="5">
+        <v>8.7438094869469907E-2</v>
+      </c>
       <c r="M3">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="N3">
         <v>5200</v>
       </c>
-      <c r="P3" s="1"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O3" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="P3" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>20</v>
       </c>
@@ -1581,24 +1640,48 @@
         <v>64</v>
       </c>
       <c r="F4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G4">
         <v>0.2</v>
       </c>
-      <c r="H4" s="6"/>
-      <c r="K4" s="8"/>
+      <c r="H4" s="6">
+        <v>0.73674242424242398</v>
+      </c>
+      <c r="I4" s="7">
+        <v>0.66422125673425902</v>
+      </c>
+      <c r="J4" s="3">
+        <v>0.148030369043952</v>
+      </c>
+      <c r="K4" s="8">
+        <v>0.71359880807259901</v>
+      </c>
+      <c r="L4" s="5">
+        <v>0.147036472263293</v>
+      </c>
       <c r="M4">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="N4">
         <v>5200</v>
       </c>
-      <c r="P4" s="1"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O4" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="P4" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="R4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="B5" t="s">
         <v>13</v>
@@ -1616,35 +1699,171 @@
         <v>2</v>
       </c>
       <c r="G5">
-        <v>0.4</v>
-      </c>
-      <c r="H5" s="6"/>
-      <c r="K5" s="8"/>
+        <v>0.2</v>
+      </c>
+      <c r="H5" s="6">
+        <v>0.84659090909090895</v>
+      </c>
+      <c r="I5" s="7">
+        <v>0.82848631306964604</v>
+      </c>
+      <c r="J5" s="3">
+        <v>6.1600314321541998E-2</v>
+      </c>
+      <c r="K5" s="8">
+        <v>0.95708096398591902</v>
+      </c>
+      <c r="L5" s="5">
+        <v>5.0051312961251503E-2</v>
+      </c>
       <c r="M5">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="N5">
         <v>5200</v>
       </c>
-      <c r="P5" s="1"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="P6" s="1"/>
-      <c r="Q6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P7" s="1"/>
-      <c r="Q7" s="24" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="P8" s="1"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="P9" s="1"/>
+      <c r="O5" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="P5" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="R5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6">
+        <v>128</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6">
+        <v>0.2</v>
+      </c>
+      <c r="H6" s="6"/>
+      <c r="K6" s="8"/>
+      <c r="M6">
+        <v>8</v>
+      </c>
+      <c r="N6">
+        <v>5200</v>
+      </c>
+      <c r="Q6" s="1"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>100</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7">
+        <v>64</v>
+      </c>
+      <c r="F7">
+        <v>4</v>
+      </c>
+      <c r="G7">
+        <v>0.2</v>
+      </c>
+      <c r="H7" s="6">
+        <v>0.84785353535353503</v>
+      </c>
+      <c r="I7" s="7">
+        <v>0.81094042989096404</v>
+      </c>
+      <c r="J7" s="3">
+        <v>6.19889095877156E-2</v>
+      </c>
+      <c r="K7" s="8">
+        <v>0.94117248849174096</v>
+      </c>
+      <c r="L7" s="5">
+        <v>5.1491779025186799E-2</v>
+      </c>
+      <c r="M7">
+        <v>8</v>
+      </c>
+      <c r="N7">
+        <v>5200</v>
+      </c>
+      <c r="O7" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="P7" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8">
+        <v>64</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8">
+        <v>0.4</v>
+      </c>
+      <c r="H8" s="6"/>
+      <c r="K8" s="8"/>
+      <c r="M8">
+        <v>8</v>
+      </c>
+      <c r="N8">
+        <v>5200</v>
+      </c>
+      <c r="Q8" s="1"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q9" s="1"/>
+    </row>
+    <row r="10" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q10" s="1"/>
+      <c r="R10" s="24"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q11" s="1"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q12" s="1"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="H1:H1048576">
@@ -1663,7 +1882,11 @@
     <cfRule type="top10" dxfId="0" priority="2" bottom="1" rank="1"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="P2" r:id="rId1" xr:uid="{06379612-5A90-48F1-A974-5BCDF9391FD0}"/>
+    <hyperlink ref="Q2" r:id="rId1" xr:uid="{29FF1DC6-6814-47C4-A793-44E2E50BC1DC}"/>
+    <hyperlink ref="Q3" r:id="rId2" xr:uid="{E47731C1-E9FA-4BD9-A706-558D99613C5B}"/>
+    <hyperlink ref="Q4" r:id="rId3" xr:uid="{6AB44BBF-FA66-45F4-B347-C46FA9CE2459}"/>
+    <hyperlink ref="Q5" r:id="rId4" xr:uid="{B0FFA28A-1D63-4009-859E-7BAB2AF7C5A6}"/>
+    <hyperlink ref="Q7" r:id="rId5" xr:uid="{F7C0A27A-2D8C-40C5-BD44-650F32FEFDDF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
addition of random transforms and multiprocess of grid mapping
</commit_message>
<xml_diff>
--- a/PROJECT/PointCould_Classification/trainings.xlsx
+++ b/PROJECT/PointCould_Classification/trainings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swann\GitHubProjects\IndividualProject\PROJECT\PointCould_Classification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECFCADB8-B477-4C5E-B24F-91F88C1B6F7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{388F8B75-1A2A-4079-BA37-C796D9143F87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-27488" yWindow="-114" windowWidth="27602" windowHeight="14899" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,6 @@
     <sheet name="KDE" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="59">
   <si>
     <t>epochs</t>
   </si>
@@ -184,6 +183,27 @@
   </si>
   <si>
     <t>results\KDE\wl_da_tt_gd=64_ks=4_epoch=100_5200_globavg</t>
+  </si>
+  <si>
+    <t>adding whitening</t>
+  </si>
+  <si>
+    <t>results\KDE\wl_da_tt_gd=64_ks=2_epoch=100_5200_globavg_whitening</t>
+  </si>
+  <si>
+    <t>6:11:8</t>
+  </si>
+  <si>
+    <t>model_globavg_deep</t>
+  </si>
+  <si>
+    <t>trying a deeper model</t>
+  </si>
+  <si>
+    <t>results\KDE\wl_da_tt_gd=64_ks=2_epoch=100_5200_globavgdeep_whitening</t>
+  </si>
+  <si>
+    <t>7:20:4</t>
   </si>
 </sst>
 </file>
@@ -1443,10 +1463,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AFD9867-B70B-41BC-9A3A-CD91040257D4}">
-  <dimension ref="A1:R12"/>
+  <dimension ref="A1:R13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12"/>
+      <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -1456,8 +1476,8 @@
     <col min="11" max="11" width="9.140625" style="9"/>
     <col min="12" max="12" width="9.140625" style="5"/>
     <col min="15" max="15" width="10.7109375" style="26" customWidth="1"/>
-    <col min="16" max="16" width="14.7109375" style="26" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="56.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.42578125" style="26" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="66" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="55" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1737,7 +1757,7 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="B6" t="s">
         <v>13</v>
@@ -1749,7 +1769,7 @@
         <v>14</v>
       </c>
       <c r="E6">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="F6">
         <v>2</v>
@@ -1757,15 +1777,39 @@
       <c r="G6">
         <v>0.2</v>
       </c>
-      <c r="H6" s="6"/>
-      <c r="K6" s="8"/>
+      <c r="H6" s="6">
+        <v>0.84406565656565602</v>
+      </c>
+      <c r="I6" s="7">
+        <v>0.82632226185517699</v>
+      </c>
+      <c r="J6" s="3">
+        <v>6.0786124619871602E-2</v>
+      </c>
+      <c r="K6" s="8">
+        <v>0.881126455456268</v>
+      </c>
+      <c r="L6" s="5">
+        <v>5.6425763218908603E-2</v>
+      </c>
       <c r="M6">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="N6">
         <v>5200</v>
       </c>
-      <c r="Q6" s="1"/>
+      <c r="O6" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="P6" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="R6" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -1822,7 +1866,7 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="B8" t="s">
         <v>13</v>
@@ -1840,30 +1884,115 @@
         <v>2</v>
       </c>
       <c r="G8">
-        <v>0.4</v>
-      </c>
-      <c r="H8" s="6"/>
-      <c r="K8" s="8"/>
+        <v>0.2</v>
+      </c>
+      <c r="H8" s="6">
+        <v>0.83901515151515105</v>
+      </c>
+      <c r="I8" s="7">
+        <v>0.82467885959482901</v>
+      </c>
+      <c r="J8" s="3">
+        <v>6.2624890281997497E-2</v>
+      </c>
+      <c r="K8" s="8">
+        <v>0.85174654752233903</v>
+      </c>
+      <c r="L8" s="5">
+        <v>5.9145503535370098E-2</v>
+      </c>
       <c r="M8">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="N8">
         <v>5200</v>
       </c>
-      <c r="Q8" s="1"/>
+      <c r="O8" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="P8" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="R8" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9">
+        <v>64</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9">
+        <v>0.4</v>
+      </c>
+      <c r="H9" s="6"/>
+      <c r="K9" s="8"/>
+      <c r="M9">
+        <v>8</v>
+      </c>
+      <c r="N9">
+        <v>5200</v>
+      </c>
       <c r="Q9" s="1"/>
     </row>
-    <row r="10" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10">
+        <v>128</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+      <c r="G10">
+        <v>0.2</v>
+      </c>
+      <c r="H10" s="6"/>
+      <c r="K10" s="8"/>
+      <c r="M10">
+        <v>8</v>
+      </c>
+      <c r="N10">
+        <v>5200</v>
+      </c>
       <c r="Q10" s="1"/>
-      <c r="R10" s="24"/>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Q11" s="1"/>
+      <c r="R11" s="24"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="Q12" s="1"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q13" s="1"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="H1:H1048576">
@@ -1885,8 +2014,10 @@
     <hyperlink ref="Q2" r:id="rId1" xr:uid="{29FF1DC6-6814-47C4-A793-44E2E50BC1DC}"/>
     <hyperlink ref="Q3" r:id="rId2" xr:uid="{E47731C1-E9FA-4BD9-A706-558D99613C5B}"/>
     <hyperlink ref="Q4" r:id="rId3" xr:uid="{6AB44BBF-FA66-45F4-B347-C46FA9CE2459}"/>
-    <hyperlink ref="Q5" r:id="rId4" xr:uid="{B0FFA28A-1D63-4009-859E-7BAB2AF7C5A6}"/>
-    <hyperlink ref="Q7" r:id="rId5" xr:uid="{F7C0A27A-2D8C-40C5-BD44-650F32FEFDDF}"/>
+    <hyperlink ref="Q7" r:id="rId4" xr:uid="{F7C0A27A-2D8C-40C5-BD44-650F32FEFDDF}"/>
+    <hyperlink ref="Q5" r:id="rId5" xr:uid="{6F362E92-4E38-433A-9651-6A629F0CE986}"/>
+    <hyperlink ref="Q6" r:id="rId6" xr:uid="{5C625378-1942-43F1-8A50-A72A0729EFC5}"/>
+    <hyperlink ref="Q8" r:id="rId7" xr:uid="{3C1B70F2-3545-4251-BD75-0473C0871CD7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
cleaning code + some trainings
</commit_message>
<xml_diff>
--- a/PROJECT/PointCould_Classification/trainings.xlsx
+++ b/PROJECT/PointCould_Classification/trainings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swann\GitHubProjects\IndividualProject\PROJECT\PointCould_Classification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{388F8B75-1A2A-4079-BA37-C796D9143F87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B456B7CD-DFF1-4BD2-A007-EFFB2E66567E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27488" yWindow="-114" windowWidth="27602" windowHeight="14899" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-114" yWindow="-114" windowWidth="27602" windowHeight="14927" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="3DmFV" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="65">
   <si>
     <t>epochs</t>
   </si>
@@ -137,9 +137,6 @@
     <t>kernel size</t>
   </si>
   <si>
-    <t>grid dim</t>
-  </si>
-  <si>
     <t>results\KDE\wl_da_tt_gd=64_ks=2_epoch=20_5200</t>
   </si>
   <si>
@@ -204,6 +201,27 @@
   </si>
   <si>
     <t>7:20:4</t>
+  </si>
+  <si>
+    <t>results\KDE\wl_tt_rt_gd=64_ks=2_epoch=100_12000_globavg_deep</t>
+  </si>
+  <si>
+    <t>transformations: rotations and scaling patches between 0.5 and 1.5</t>
+  </si>
+  <si>
+    <t>11:22:29</t>
+  </si>
+  <si>
+    <t>results\KDE\wl_tt_rt_gd=64_ks=2_epoch=100_12000_globavg_deep_noscaling</t>
+  </si>
+  <si>
+    <t>transformations: rotations and no scaling</t>
+  </si>
+  <si>
+    <t>grid size</t>
+  </si>
+  <si>
+    <t>11:7:3</t>
   </si>
 </sst>
 </file>
@@ -721,7 +739,7 @@
   <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -1466,7 +1484,7 @@
   <dimension ref="A1:R13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q18" sqref="Q18"/>
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -1478,7 +1496,7 @@
     <col min="15" max="15" width="10.7109375" style="26" customWidth="1"/>
     <col min="16" max="16" width="20.42578125" style="26" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="66" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="55" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="88.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="10" customFormat="1" ht="42.8" x14ac:dyDescent="0.25">
@@ -1495,13 +1513,13 @@
         <v>1</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>36</v>
+        <v>63</v>
       </c>
       <c r="F1" s="10" t="s">
         <v>35</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H1" s="11" t="s">
         <v>5</v>
@@ -1528,7 +1546,7 @@
         <v>22</v>
       </c>
       <c r="P1" s="25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Q1" s="10" t="s">
         <v>10</v>
@@ -1581,13 +1599,13 @@
         <v>5200</v>
       </c>
       <c r="O2" s="26" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P2" s="26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -1634,13 +1652,13 @@
         <v>5200</v>
       </c>
       <c r="O3" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P3" s="26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -1687,16 +1705,16 @@
         <v>5200</v>
       </c>
       <c r="O4" s="26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P4" s="26" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -1743,16 +1761,16 @@
         <v>5200</v>
       </c>
       <c r="O5" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="P5" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q5" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="P5" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q5" s="1" t="s">
+      <c r="R5" t="s">
         <v>49</v>
-      </c>
-      <c r="R5" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -1799,16 +1817,16 @@
         <v>5200</v>
       </c>
       <c r="O6" s="26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="P6" s="26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="R6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -1855,13 +1873,13 @@
         <v>5200</v>
       </c>
       <c r="O7" s="26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="P7" s="26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -1908,16 +1926,16 @@
         <v>5200</v>
       </c>
       <c r="O8" s="26" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="P8" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="R8" t="s">
         <v>55</v>
-      </c>
-      <c r="Q8" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="R8" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -1942,8 +1960,6 @@
       <c r="G9">
         <v>0.4</v>
       </c>
-      <c r="H9" s="6"/>
-      <c r="K9" s="8"/>
       <c r="M9">
         <v>8</v>
       </c>
@@ -1985,29 +2001,134 @@
       <c r="Q10" s="1"/>
     </row>
     <row r="11" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="Q11" s="1"/>
-      <c r="R11" s="24"/>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="Q12" s="1"/>
+      <c r="A11">
+        <v>100</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11">
+        <v>64</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+      <c r="G11">
+        <v>0.2</v>
+      </c>
+      <c r="H11" s="6">
+        <v>0.83818770226537198</v>
+      </c>
+      <c r="I11" s="7">
+        <v>0.84311744335167005</v>
+      </c>
+      <c r="J11" s="3">
+        <v>6.1002034159609503E-2</v>
+      </c>
+      <c r="K11" s="8">
+        <v>0.85037262872628705</v>
+      </c>
+      <c r="L11" s="5">
+        <v>5.8830085652163203E-2</v>
+      </c>
+      <c r="M11">
+        <v>12</v>
+      </c>
+      <c r="N11">
+        <v>12000</v>
+      </c>
+      <c r="O11" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="P11" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="R11" s="24" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>100</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12">
+        <v>64</v>
+      </c>
+      <c r="F12">
+        <v>2</v>
+      </c>
+      <c r="G12">
+        <v>0.2</v>
+      </c>
+      <c r="H12" s="6">
+        <v>0.83818770226537198</v>
+      </c>
+      <c r="I12" s="7">
+        <v>0.83681911908084206</v>
+      </c>
+      <c r="J12" s="3">
+        <v>6.0942197901986503E-2</v>
+      </c>
+      <c r="K12" s="8">
+        <v>0.84457994579945705</v>
+      </c>
+      <c r="L12" s="5">
+        <v>5.9482747623563398E-2</v>
+      </c>
+      <c r="M12">
+        <v>12</v>
+      </c>
+      <c r="N12">
+        <v>12000</v>
+      </c>
+      <c r="O12" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="P12" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="R12" s="24" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="Q13" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="H1:H1048576">
+  <conditionalFormatting sqref="H1:H8 H10:H1048576">
     <cfRule type="top10" dxfId="4" priority="5" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I1:I1048576">
+  <conditionalFormatting sqref="I1:I8 I10:I1048576">
     <cfRule type="top10" dxfId="3" priority="4" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J1:J1048576">
+  <conditionalFormatting sqref="J1:J8 J10:J1048576">
     <cfRule type="top10" dxfId="2" priority="3" bottom="1" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K1:K1048576">
+  <conditionalFormatting sqref="K1:K8 K10:K1048576">
     <cfRule type="top10" dxfId="1" priority="1" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L1:L1048576">
+  <conditionalFormatting sqref="L1:L8 L10:L1048576">
     <cfRule type="top10" dxfId="0" priority="2" bottom="1" rank="1"/>
   </conditionalFormatting>
   <hyperlinks>
@@ -2018,6 +2139,8 @@
     <hyperlink ref="Q5" r:id="rId5" xr:uid="{6F362E92-4E38-433A-9651-6A629F0CE986}"/>
     <hyperlink ref="Q6" r:id="rId6" xr:uid="{5C625378-1942-43F1-8A50-A72A0729EFC5}"/>
     <hyperlink ref="Q8" r:id="rId7" xr:uid="{3C1B70F2-3545-4251-BD75-0473C0871CD7}"/>
+    <hyperlink ref="Q11" r:id="rId8" xr:uid="{99B8080F-6E56-4F77-BF77-D7B28AAF79C0}"/>
+    <hyperlink ref="Q12" r:id="rId9" xr:uid="{CCF8A742-6B9F-4401-83F5-C34F8223F5FC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
training from pretrained model implementation
</commit_message>
<xml_diff>
--- a/PROJECT/PointCould_Classification/trainings.xlsx
+++ b/PROJECT/PointCould_Classification/trainings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swann\GitHubProjects\IndividualProject\PROJECT\PointCould_Classification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B456B7CD-DFF1-4BD2-A007-EFFB2E66567E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D722CC1-0BB0-45FB-9D6D-A7023A80917D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-114" yWindow="-114" windowWidth="27602" windowHeight="14927" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="69">
   <si>
     <t>epochs</t>
   </si>
@@ -222,6 +222,18 @@
   </si>
   <si>
     <t>11:7:3</t>
+  </si>
+  <si>
+    <t>13:15:6</t>
+  </si>
+  <si>
+    <t>results\KDE\wl_tt_rt_gd=128_ks=2_epoch=20_12000_globavg_deep</t>
+  </si>
+  <si>
+    <t>results\KDE\wl_tt_gd=64_ks=2_epoch=100_12000_globavg_deep</t>
+  </si>
+  <si>
+    <t>10:39:14</t>
   </si>
 </sst>
 </file>
@@ -1481,10 +1493,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AFD9867-B70B-41BC-9A3A-CD91040257D4}">
-  <dimension ref="A1:R13"/>
+  <dimension ref="A1:R12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -1946,43 +1958,66 @@
         <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E9">
-        <v>64</v>
+        <v>128</v>
       </c>
       <c r="F9">
         <v>2</v>
       </c>
       <c r="G9">
-        <v>0.4</v>
+        <v>0.2</v>
+      </c>
+      <c r="H9" s="6">
+        <v>0.76107273466070702</v>
+      </c>
+      <c r="I9" s="7">
+        <v>0.58330835354893196</v>
+      </c>
+      <c r="J9" s="3">
+        <v>0.79325023561122698</v>
+      </c>
+      <c r="K9" s="8">
+        <v>0.75083867032631901</v>
+      </c>
+      <c r="L9" s="5">
+        <v>0.80232993433288102</v>
       </c>
       <c r="M9">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="N9">
         <v>5200</v>
       </c>
-      <c r="Q9" s="1"/>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="O9" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="P9" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="B10" t="s">
         <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E10">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="F10">
         <v>2</v>
@@ -1990,15 +2025,39 @@
       <c r="G10">
         <v>0.2</v>
       </c>
-      <c r="H10" s="6"/>
-      <c r="K10" s="8"/>
+      <c r="H10" s="6">
+        <v>0.83818770226537198</v>
+      </c>
+      <c r="I10" s="7">
+        <v>0.84311744335167005</v>
+      </c>
+      <c r="J10" s="3">
+        <v>6.1002034159609503E-2</v>
+      </c>
+      <c r="K10" s="8">
+        <v>0.85037262872628705</v>
+      </c>
+      <c r="L10" s="5">
+        <v>5.8830085652163203E-2</v>
+      </c>
       <c r="M10">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="N10">
-        <v>5200</v>
-      </c>
-      <c r="Q10" s="1"/>
+        <v>12000</v>
+      </c>
+      <c r="O10" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="P10" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="R10" s="24" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="11" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -2026,16 +2085,16 @@
         <v>0.83818770226537198</v>
       </c>
       <c r="I11" s="7">
-        <v>0.84311744335167005</v>
+        <v>0.83681911908084206</v>
       </c>
       <c r="J11" s="3">
-        <v>6.1002034159609503E-2</v>
+        <v>6.0942197901986503E-2</v>
       </c>
       <c r="K11" s="8">
-        <v>0.85037262872628705</v>
+        <v>0.84457994579945705</v>
       </c>
       <c r="L11" s="5">
-        <v>5.8830085652163203E-2</v>
+        <v>5.9482747623563398E-2</v>
       </c>
       <c r="M11">
         <v>12</v>
@@ -2044,16 +2103,16 @@
         <v>12000</v>
       </c>
       <c r="O11" s="26" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="P11" s="26" t="s">
         <v>54</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="R11" s="24" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2067,7 +2126,7 @@
         <v>14</v>
       </c>
       <c r="D12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E12">
         <v>64</v>
@@ -2079,19 +2138,19 @@
         <v>0.2</v>
       </c>
       <c r="H12" s="6">
-        <v>0.83818770226537198</v>
+        <v>0.83495145631067902</v>
       </c>
       <c r="I12" s="7">
-        <v>0.83681911908084206</v>
+        <v>0.80448186425355195</v>
       </c>
       <c r="J12" s="3">
-        <v>6.0942197901986503E-2</v>
+        <v>6.2196001828273798E-2</v>
       </c>
       <c r="K12" s="8">
-        <v>0.84457994579945705</v>
+        <v>0.92533875338753302</v>
       </c>
       <c r="L12" s="5">
-        <v>5.9482747623563398E-2</v>
+        <v>5.2519237763685098E-2</v>
       </c>
       <c r="M12">
         <v>12</v>
@@ -2100,35 +2159,30 @@
         <v>12000</v>
       </c>
       <c r="O12" s="26" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="P12" s="26" t="s">
         <v>54</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="R12" s="24" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="Q13" s="1"/>
+        <v>67</v>
+      </c>
+      <c r="R12" s="24"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="H1:H8 H10:H1048576">
+  <conditionalFormatting sqref="H1:H1048576">
     <cfRule type="top10" dxfId="4" priority="5" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I1:I8 I10:I1048576">
+  <conditionalFormatting sqref="I1:I1048576">
     <cfRule type="top10" dxfId="3" priority="4" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J1:J8 J10:J1048576">
+  <conditionalFormatting sqref="J1:J1048576">
     <cfRule type="top10" dxfId="2" priority="3" bottom="1" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K1:K8 K10:K1048576">
+  <conditionalFormatting sqref="K1:K1048576">
     <cfRule type="top10" dxfId="1" priority="1" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L1:L8 L10:L1048576">
+  <conditionalFormatting sqref="L1:L1048576">
     <cfRule type="top10" dxfId="0" priority="2" bottom="1" rank="1"/>
   </conditionalFormatting>
   <hyperlinks>
@@ -2139,8 +2193,10 @@
     <hyperlink ref="Q5" r:id="rId5" xr:uid="{6F362E92-4E38-433A-9651-6A629F0CE986}"/>
     <hyperlink ref="Q6" r:id="rId6" xr:uid="{5C625378-1942-43F1-8A50-A72A0729EFC5}"/>
     <hyperlink ref="Q8" r:id="rId7" xr:uid="{3C1B70F2-3545-4251-BD75-0473C0871CD7}"/>
-    <hyperlink ref="Q11" r:id="rId8" xr:uid="{99B8080F-6E56-4F77-BF77-D7B28AAF79C0}"/>
-    <hyperlink ref="Q12" r:id="rId9" xr:uid="{CCF8A742-6B9F-4401-83F5-C34F8223F5FC}"/>
+    <hyperlink ref="Q10" r:id="rId8" xr:uid="{99B8080F-6E56-4F77-BF77-D7B28AAF79C0}"/>
+    <hyperlink ref="Q11" r:id="rId9" xr:uid="{CCF8A742-6B9F-4401-83F5-C34F8223F5FC}"/>
+    <hyperlink ref="Q9" r:id="rId10" xr:uid="{11114837-BDBF-4791-8624-4644E3DE6C2F}"/>
+    <hyperlink ref="Q12" r:id="rId11" xr:uid="{C8593669-0451-496A-9FE1-C8692B2BA35F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>